<commit_message>
Updated status for 20th April- Pratiksha and me
</commit_message>
<xml_diff>
--- a/Daily Status update Report 20042020.xlsx
+++ b/Daily Status update Report 20042020.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1101" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1103" uniqueCount="182">
   <si>
     <t>Sr.No</t>
   </si>
@@ -576,6 +576,15 @@
   </si>
   <si>
     <t>Prepared test scenarios for SO</t>
+  </si>
+  <si>
+    <t>1.Completed with Test Cases Writing for Collateral Deposit Cash - Checked-Checked- Security Deposit Scenario
+(for a. Created-&gt;Accepted-&gt; Settled
+b. Created-&gt;Accepted-&gt; Manually Settled)
+2. Discussed with Pruthvi on what Testcases should be included to cover CD284 broadcast message</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prepared test cases for normal trade flow; Preparing test cases for rectified trade flow(1st 3 broadcast messages completed) </t>
   </si>
 </sst>
 </file>
@@ -49520,7 +49529,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
@@ -49937,7 +49946,7 @@
       <c r="Y10" s="24"/>
       <c r="Z10" s="24"/>
     </row>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1">
+    <row r="11" spans="1:26" ht="90">
       <c r="A11" s="25">
         <v>10</v>
       </c>
@@ -49956,7 +49965,9 @@
       <c r="F11" s="40">
         <v>0.75</v>
       </c>
-      <c r="G11" s="38"/>
+      <c r="G11" s="38" t="s">
+        <v>180</v>
+      </c>
       <c r="H11" s="24"/>
       <c r="I11" s="24"/>
       <c r="J11" s="24"/>
@@ -49977,7 +49988,7 @@
       <c r="Y11" s="24"/>
       <c r="Z11" s="24"/>
     </row>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1">
+    <row r="12" spans="1:26" ht="30">
       <c r="A12" s="25">
         <v>11</v>
       </c>
@@ -49991,12 +50002,14 @@
         <v>8</v>
       </c>
       <c r="E12" s="36">
-        <v>0.38194444444444442</v>
+        <v>0.375</v>
       </c>
       <c r="F12" s="40">
-        <v>0.74652777777777779</v>
-      </c>
-      <c r="G12" s="38"/>
+        <v>0.73958333333333337</v>
+      </c>
+      <c r="G12" s="38" t="s">
+        <v>181</v>
+      </c>
       <c r="H12" s="24"/>
       <c r="I12" s="24"/>
       <c r="J12" s="24"/>

</xml_diff>

<commit_message>
status updated for 20th april
</commit_message>
<xml_diff>
--- a/Daily Status update Report 20042020.xlsx
+++ b/Daily Status update Report 20042020.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1103" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1104" uniqueCount="183">
   <si>
     <t>Sr.No</t>
   </si>
@@ -585,6 +585,9 @@
   </si>
   <si>
     <t xml:space="preserve">Prepared test cases for normal trade flow; Preparing test cases for rectified trade flow(1st 3 broadcast messages completed) </t>
+  </si>
+  <si>
+    <t>Tosca Installation and Setup ; Started with the orange hrms automation</t>
   </si>
 </sst>
 </file>
@@ -49529,7 +49532,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
@@ -50049,7 +50052,9 @@
       <c r="F13" s="37">
         <v>0.75</v>
       </c>
-      <c r="G13" s="41"/>
+      <c r="G13" s="41" t="s">
+        <v>182</v>
+      </c>
       <c r="H13" s="24"/>
       <c r="I13" s="24"/>
       <c r="J13" s="24"/>

</xml_diff>

<commit_message>
Status for 20th April-NFT
</commit_message>
<xml_diff>
--- a/Daily Status update Report 20042020.xlsx
+++ b/Daily Status update Report 20042020.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1104" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1105" uniqueCount="184">
   <si>
     <t>Sr.No</t>
   </si>
@@ -588,6 +588,9 @@
   </si>
   <si>
     <t>Tosca Installation and Setup ; Started with the orange hrms automation</t>
+  </si>
+  <si>
+    <t>Working on PPT and "Test execution plan" for PT</t>
   </si>
 </sst>
 </file>
@@ -49532,7 +49535,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
@@ -49928,7 +49931,9 @@
       <c r="F10" s="37">
         <v>0.77083333333333337</v>
       </c>
-      <c r="G10" s="39"/>
+      <c r="G10" s="39" t="s">
+        <v>183</v>
+      </c>
       <c r="H10" s="24"/>
       <c r="I10" s="24"/>
       <c r="J10" s="24"/>

</xml_diff>